<commit_message>
fixed the bug for TLB overflow and TLB busy write/red address, added intermittent software benchmarksand results
</commit_message>
<xml_diff>
--- a/benchmark/assesment/benchmark.xlsx
+++ b/benchmark/assesment/benchmark.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="component overhead" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Original C" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Qwark Bitcount" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Qwark AR" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Qwark Cuckoo" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t xml:space="preserve">System Checkpoint</t>
   </si>
@@ -98,10 +101,10 @@
     <t xml:space="preserve">Optimization</t>
   </si>
   <si>
-    <t xml:space="preserve">Time on MSP430FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time on MSP430G2</t>
+    <t xml:space="preserve">Time on MSP430FR5969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time on MSP430G2553</t>
   </si>
   <si>
     <t xml:space="preserve">Time on OpenMSP430</t>
@@ -119,6 +122,9 @@
     <t xml:space="preserve">282.032 ms</t>
   </si>
   <si>
+    <t xml:space="preserve">Does not Fit</t>
+  </si>
+  <si>
     <t xml:space="preserve">248.71ms</t>
   </si>
   <si>
@@ -128,6 +134,9 @@
     <t xml:space="preserve">207.116 ms</t>
   </si>
   <si>
+    <t xml:space="preserve">170.3038 ms</t>
+  </si>
+  <si>
     <t xml:space="preserve">177.40ms</t>
   </si>
   <si>
@@ -137,51 +146,42 @@
     <t xml:space="preserve">194.295 ms</t>
   </si>
   <si>
+    <t xml:space="preserve">163.079 ms</t>
+  </si>
+  <si>
     <t xml:space="preserve">170.469 ms</t>
   </si>
   <si>
-    <t xml:space="preserve">O3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93.647 ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.97 ms</t>
-  </si>
-  <si>
     <t xml:space="preserve">AR</t>
   </si>
   <si>
     <t xml:space="preserve">4.346813 s</t>
   </si>
   <si>
-    <t xml:space="preserve">3.921396625 s</t>
+    <t xml:space="preserve">3.420297 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.921 s</t>
   </si>
   <si>
     <t xml:space="preserve">2.365221 s</t>
   </si>
   <si>
+    <t xml:space="preserve">1.814630 s</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.089016 s</t>
   </si>
   <si>
-    <t xml:space="preserve">volatile and global works equally well for O1</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.348716 s</t>
   </si>
   <si>
+    <t xml:space="preserve">1.859374 s</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.030978 s</t>
   </si>
   <si>
-    <t xml:space="preserve">volatile doesnt work for O2/O3 so global</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.248858 s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.945140 s</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cuckoo</t>
   </si>
   <si>
@@ -203,18 +203,34 @@
     <t xml:space="preserve">11.781125 ms</t>
   </si>
   <si>
-    <t xml:space="preserve">14.156 ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.518 ms</t>
+    <t xml:space="preserve">Cycles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overhead compared with Original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Buffer Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write Buffer Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLB buffer Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -484,7 +500,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,6 +547,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -641,7 +661,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,10 +922,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A6:J23"/>
+  <dimension ref="A6:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -913,9 +933,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="48.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.53"/>
   </cols>
   <sheetData>
@@ -925,244 +945,234 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="E12" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="F12" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="D13" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="E13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="B14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="D14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>41</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="E16" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="F16" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="E17" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="F17" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="E18" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="F18" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="0" t="s">
+      <c r="E20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="0" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="0" t="s">
+      <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1177,4 +1187,466 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:J4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>294209</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>294.209625</v>
+      </c>
+      <c r="G2" s="12" t="n">
+        <v>0.1825</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>225256</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>225.25625</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>0.2698</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>221778</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>221.778</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:J4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>3941097</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>3.941</v>
+      </c>
+      <c r="G2" s="12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>3148101</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>3.148</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>0.1569</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>3249480</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>3.249</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:J5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>327552</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>327.552</v>
+      </c>
+      <c r="G2" s="12" t="n">
+        <v>0.1033</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>53524</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>53.524</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>0.1246</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>21246</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>21.246</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>0.1803</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>